<commit_message>
Added recursive loading for multiple xlsx files
</commit_message>
<xml_diff>
--- a/maps/data/ED42_Unofficial.xlsx
+++ b/maps/data/ED42_Unofficial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\Election-Mapbox-Local\maps\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C78EE34-57FD-4FA7-B70B-E1DFEF2A83C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D3DD20-A016-4766-BE34-920A5C9AD8D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5355" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,9 +561,7 @@
   </sheetPr>
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>